<commit_message>
Update BO templates with new B29 cell for Net excl SLA
- Updated both Backlite and Viola BO templates
- Added B29 cell for Net excl SLA value (matching template change)
- Templates now support new location splits format in A33

🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/bo_templates/backlite_bo_template.xlsx
+++ b/bo_templates/backlite_bo_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\97158\Backlite Media Dropbox\Sales\Booking Order Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amrtamer711/Documents/Sales Proposals/bo_templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BC4E0F-AEA1-4CD1-A334-8D4543D3AF12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19EC805-6551-3642-B3B2-57BE25513D20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{30FAD0CB-2E7E-4CA9-A11C-3C1D7AE234D8}"/>
+    <workbookView xWindow="-120" yWindow="680" windowWidth="29040" windowHeight="15720" xr2:uid="{30FAD0CB-2E7E-4CA9-A11C-3C1D7AE234D8}"/>
   </bookViews>
   <sheets>
     <sheet name="BO Form" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Booking Order Form</t>
   </si>
@@ -105,7 +105,10 @@
     <t>Net excl. VAT:</t>
   </si>
   <si>
-    <t>Net rentals excl. SLA:</t>
+    <t>Net excl. SLA:</t>
+  </si>
+  <si>
+    <t>Location splits excl. SLA:</t>
   </si>
 </sst>
 </file>
@@ -497,9 +500,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -537,7 +540,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -643,7 +646,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -785,7 +788,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -799,20 +802,20 @@
   <dimension ref="A9:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="A32" sqref="A32:E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="42.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="3.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="21.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="3.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="2" customWidth="1"/>
     <col min="5" max="5" width="38" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.85546875" style="2"/>
+    <col min="6" max="16384" width="8.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>0</v>
       </c>
@@ -823,11 +826,11 @@
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:7" ht="38.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="38.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>1</v>
       </c>
@@ -837,12 +840,12 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="6"/>
       <c r="D12" s="7"/>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:7" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="33.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>2</v>
       </c>
@@ -852,12 +855,12 @@
       </c>
       <c r="E13" s="14"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="6"/>
       <c r="D14" s="7"/>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="31.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>5</v>
       </c>
@@ -867,12 +870,12 @@
       </c>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="6"/>
       <c r="D16" s="7"/>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="8" t="s">
         <v>6</v>
       </c>
@@ -882,12 +885,12 @@
       </c>
       <c r="E17" s="14"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="6"/>
       <c r="D18" s="7"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="32.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="8" t="s">
         <v>21</v>
       </c>
@@ -897,13 +900,13 @@
       </c>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="D20" s="7"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>9</v>
       </c>
@@ -915,13 +918,13 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="6"/>
       <c r="B22" s="19"/>
       <c r="C22" s="7"/>
       <c r="E22" s="7"/>
     </row>
-    <row r="23" spans="1:5" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>20</v>
       </c>
@@ -935,12 +938,12 @@
         <v>18</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="16"/>
       <c r="E24" s="5"/>
     </row>
-    <row r="25" spans="1:5" ht="23.65" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="23.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>10</v>
       </c>
@@ -950,11 +953,11 @@
       </c>
       <c r="E25" s="3"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D26" s="17"/>
       <c r="E26" s="5"/>
     </row>
-    <row r="27" spans="1:5" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>24</v>
       </c>
@@ -964,81 +967,83 @@
       </c>
       <c r="E27" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="20"/>
       <c r="B28" s="16"/>
       <c r="E28" s="5"/>
     </row>
-    <row r="29" spans="1:5" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="16"/>
-      <c r="B29" s="16"/>
+    <row r="29" spans="1:5" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="15"/>
       <c r="D29" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E29" s="23"/>
     </row>
-    <row r="30" spans="1:5" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="23.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="21"/>
       <c r="B30" s="16"/>
       <c r="D30" s="7"/>
       <c r="E30" s="20"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="22"/>
       <c r="E31" s="22"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="27" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B32" s="28"/>
       <c r="C32" s="28"/>
       <c r="D32" s="28"/>
       <c r="E32" s="29"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="30"/>
       <c r="B33" s="31"/>
       <c r="C33" s="31"/>
       <c r="D33" s="31"/>
       <c r="E33" s="32"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="30"/>
       <c r="B34" s="31"/>
       <c r="C34" s="31"/>
       <c r="D34" s="31"/>
       <c r="E34" s="32"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="30"/>
       <c r="B35" s="31"/>
       <c r="C35" s="31"/>
       <c r="D35" s="31"/>
       <c r="E35" s="32"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="30"/>
       <c r="B36" s="31"/>
       <c r="C36" s="31"/>
       <c r="D36" s="31"/>
       <c r="E36" s="32"/>
     </row>
-    <row r="37" spans="1:5" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="33"/>
       <c r="B37" s="34"/>
       <c r="C37" s="34"/>
       <c r="D37" s="34"/>
       <c r="E37" s="35"/>
     </row>
-    <row r="38" spans="1:5" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="36"/>
       <c r="B38" s="37"/>
       <c r="C38" s="37"/>
       <c r="D38" s="37"/>
       <c r="E38" s="37"/>
     </row>
-    <row r="39" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>22</v>
       </c>
@@ -1047,19 +1052,19 @@
       <c r="D39" s="37"/>
       <c r="E39" s="38"/>
     </row>
-    <row r="42" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>15</v>
       </c>
       <c r="B42" s="3"/>
     </row>
-    <row r="43" spans="1:5" ht="25.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B43" s="12"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E46" s="13" t="s">
         <v>17</v>
       </c>

</xml_diff>